<commit_message>
adjust xticks, yticks and size of figures, add normalized throughput
</commit_message>
<xml_diff>
--- a/src/Data/Scalability/CluStream/Clustream-Dimension-KDD98-Latency-xParallelism.xlsx
+++ b/src/Data/Scalability/CluStream/Clustream-Dimension-KDD98-Latency-xParallelism.xlsx
@@ -57,27 +57,27 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>D=50</t>
+    <t>#features=50</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>D=100</t>
+    <t>#features=100</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>D=150</t>
+    <t>#features=150</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>D=200</t>
+    <t>#features=200</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>D=250</t>
+    <t>#features=250</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>D=315</t>
+    <t>#features=315</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -253,10 +253,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>D=250</c:v>
+                  <c:v>#features=250</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>D=315</c:v>
+                  <c:v>#features=315</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -281,7 +281,7 @@
               <c15:filteredSeriesTitle>
                 <c15:tx>
                   <c:strRef>
-                    <c:extLst xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart">
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!#REF!</c15:sqref>
@@ -319,10 +319,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>D=250</c:v>
+                  <c:v>#features=250</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>D=315</c:v>
+                  <c:v>#features=315</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -347,7 +347,7 @@
               <c15:filteredSeriesTitle>
                 <c15:tx>
                   <c:strRef>
-                    <c:extLst xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart">
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!#REF!</c15:sqref>
@@ -385,10 +385,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>D=250</c:v>
+                  <c:v>#features=250</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>D=315</c:v>
+                  <c:v>#features=315</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -416,7 +416,7 @@
               <c15:filteredSeriesTitle>
                 <c15:tx>
                   <c:strRef>
-                    <c:extLst xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart">
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!#REF!</c15:sqref>
@@ -454,10 +454,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>D=250</c:v>
+                  <c:v>#features=250</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>D=315</c:v>
+                  <c:v>#features=315</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -485,7 +485,7 @@
               <c15:filteredSeriesTitle>
                 <c15:tx>
                   <c:strRef>
-                    <c:extLst xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart">
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!#REF!</c15:sqref>
@@ -523,10 +523,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>D=250</c:v>
+                  <c:v>#features=250</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>D=315</c:v>
+                  <c:v>#features=315</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -554,7 +554,7 @@
               <c15:filteredSeriesTitle>
                 <c15:tx>
                   <c:strRef>
-                    <c:extLst xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart">
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!#REF!</c15:sqref>
@@ -592,10 +592,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>D=250</c:v>
+                  <c:v>#features=250</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>D=315</c:v>
+                  <c:v>#features=315</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -623,7 +623,7 @@
               <c15:filteredSeriesTitle>
                 <c15:tx>
                   <c:strRef>
-                    <c:extLst xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart">
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!#REF!</c15:sqref>
@@ -652,11 +652,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1066046032"/>
-        <c:axId val="-1066044256"/>
+        <c:axId val="-1508745696"/>
+        <c:axId val="-1517989136"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1066046032"/>
+        <c:axId val="-1508745696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -699,7 +699,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1066044256"/>
+        <c:crossAx val="-1517989136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -707,7 +707,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1066044256"/>
+        <c:axId val="-1517989136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -758,7 +758,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1066046032"/>
+        <c:crossAx val="-1508745696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1401,7 +1401,7 @@
         <xdr:cNvPr id="5" name="图表 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3ADF420E-CB11-B149-AC71-0BFF72A073B4}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3ADF420E-CB11-B149-AC71-0BFF72A073B4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>

</xml_diff>